<commit_message>
Minor fix for temp files in optimisation mode.
</commit_message>
<xml_diff>
--- a/xlsxwriter/test/comparison/xlsx_files/optimize11.xlsx
+++ b/xlsxwriter/test/comparison/xlsx_files/optimize11.xlsx
@@ -16,7 +16,6 @@
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
     <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
     <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
-    <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -349,7 +348,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -358,27 +357,21 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Hello world</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Hello world</t>
+          <t>Hello 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Hello 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hello 3</t>
         </is>
       </c>
     </row>
@@ -389,16 +382,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Hello world</t>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Hello 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Hello 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hello 3</t>
         </is>
       </c>
     </row>
@@ -409,16 +416,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Hello world</t>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Hello 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Hello 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hello 3</t>
         </is>
       </c>
     </row>
@@ -429,16 +450,30 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Hello world</t>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Hello 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Hello 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hello 3</t>
         </is>
       </c>
     </row>
@@ -449,16 +484,30 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Hello world</t>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Hello 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Hello 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hello 3</t>
         </is>
       </c>
     </row>
@@ -469,16 +518,30 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Hello world</t>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Hello 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Hello 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hello 3</t>
         </is>
       </c>
     </row>
@@ -489,16 +552,30 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Hello world</t>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Hello 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Hello 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hello 3</t>
         </is>
       </c>
     </row>
@@ -509,16 +586,30 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Hello world</t>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Hello 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Hello 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hello 3</t>
         </is>
       </c>
     </row>
@@ -529,16 +620,30 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Hello world</t>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Hello 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Hello 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hello 3</t>
         </is>
       </c>
     </row>

</xml_diff>